<commit_message>
Planilha de requisitos + modelo Lógico de BD
</commit_message>
<xml_diff>
--- a/dmrr_matriz_requisitos.xlsx
+++ b/dmrr_matriz_requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARQUIVOS\2-sem\projeto-inovacao\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raissa Domingos\Desktop\ProjetoGit_Remoto\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FAE8B3-6CCD-411C-B6BC-22D1432B33E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBDC59E-B151-4963-B725-E072AB6C58F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Histórico de Alterações" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="102">
   <si>
     <t>Proposto</t>
   </si>
@@ -284,24 +284,15 @@
     <t>Cadastrar dados do sistema</t>
   </si>
   <si>
-    <t>Alertas dos dispositivos em risco</t>
-  </si>
-  <si>
     <t>1.4</t>
   </si>
   <si>
-    <t>Monitora se cameras estão ligadas/ativas</t>
-  </si>
-  <si>
     <t>1.5</t>
   </si>
   <si>
     <t>Cadastrar dados dos dispositivos do sistema de segurança</t>
   </si>
   <si>
-    <t>Armazenar logs do desempenhos dos dispositvos</t>
-  </si>
-  <si>
     <t>Projeto: securIT: Monitoramento de Sistemas de Segurança</t>
   </si>
   <si>
@@ -311,15 +302,9 @@
     <t>Importante</t>
   </si>
   <si>
-    <t>Rápidez de Alerta</t>
-  </si>
-  <si>
     <t>Tela de Login</t>
   </si>
   <si>
-    <t>Relatórios de análise do sistema</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -329,27 +314,9 @@
     <t>Sistema Resiliente</t>
   </si>
   <si>
-    <t>API para acesso aos dispositivos</t>
-  </si>
-  <si>
     <t>Cadastro e Seleção de componentes que serão monitorados</t>
   </si>
   <si>
-    <t>envio de notificações slack ou outro</t>
-  </si>
-  <si>
-    <t>abertura de chamado</t>
-  </si>
-  <si>
-    <t>captura de logs para compor chamado</t>
-  </si>
-  <si>
-    <t>analise dos chamados</t>
-  </si>
-  <si>
-    <t>responsivo</t>
-  </si>
-  <si>
     <t>usabilidade</t>
   </si>
   <si>
@@ -365,20 +332,137 @@
     <t>Monitorar de dispositivos de Sistemas de Segurança</t>
   </si>
   <si>
-    <t>Monitora acessos prédio/sistema/computadores (?)</t>
-  </si>
-  <si>
-    <t>Tela de Dashboard com Gráficos com a média</t>
-  </si>
-  <si>
-    <t>Persistência de registros a cada xx seg</t>
+    <t>Monitorar status dos dispositivos</t>
+  </si>
+  <si>
+    <t>Monitorar acesso ao sistema</t>
+  </si>
+  <si>
+    <t>Conter tela de Dashboard com Gráficos com a média</t>
+  </si>
+  <si>
+    <t>Emitir alertas dos dispositivos em níveis críticos</t>
+  </si>
+  <si>
+    <t>Armazenar logs do desempenho dos dispositvos</t>
+  </si>
+  <si>
+    <t>Agilidade na exibição de alertas</t>
+  </si>
+  <si>
+    <t>Relatórios contendo a análise estatística do sistema</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>Escolher servidor web para hospedagem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicar a base de dados </t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>Realizar Backup semanal</t>
+  </si>
+  <si>
+    <t>Deve ser responsivo</t>
+  </si>
+  <si>
+    <t>Realizar analise dos chamados</t>
+  </si>
+  <si>
+    <t>Habilitar a abertura de chamados</t>
+  </si>
+  <si>
+    <t>Enviar notificações via slack ou outro</t>
+  </si>
+  <si>
+    <t>Persistência de registros a cada 10 seg</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Máxima</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>Gerson</t>
+  </si>
+  <si>
+    <t>Criar API para acesso aos dispositivos</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Autenticar o usuário no sistema</t>
+  </si>
+  <si>
+    <t>Mostrar a média de forma intuitiva</t>
+  </si>
+  <si>
+    <t>Mostrar os registros em tempo real</t>
+  </si>
+  <si>
+    <t>Alertar usuário sobre uma anormalidade</t>
+  </si>
+  <si>
+    <t>Exibir os alertas no menor tempo possível</t>
+  </si>
+  <si>
+    <t>Utilizar logs para compor chamado</t>
+  </si>
+  <si>
+    <t>Servidor de Hospedagem</t>
+  </si>
+  <si>
+    <t>Dispositivos</t>
+  </si>
+  <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>Ferramenta de SDK</t>
+  </si>
+  <si>
+    <t>Raissa</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>Fernanda</t>
+  </si>
+  <si>
+    <t>Matheus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -895,7 +979,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1116,6 +1200,15 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1617,8 +1710,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="D7:U75" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
-  <autoFilter ref="D7:U75" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="D7:U79" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="D7:U79" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descrição do Requisito" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
@@ -1970,7 +2063,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
@@ -1981,7 +2074,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="12.75" customHeight="1">
+    <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="57" t="s">
         <v>17</v>
       </c>
@@ -1989,7 +2082,7 @@
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
     </row>
-    <row r="4" spans="2:5" ht="27" customHeight="1">
+    <row r="4" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -2003,7 +2096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15">
+    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
@@ -2013,49 +2106,49 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:5" ht="15">
+    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:5" ht="15">
+    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:5" ht="15">
+    <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:5" ht="15">
+    <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:5" ht="15">
+    <row r="10" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:5" ht="15">
+    <row r="11" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:5" ht="15">
+    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>19</v>
       </c>
@@ -2063,12 +2156,12 @@
         <v>41293</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15" customHeight="1">
+    <row r="39" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>31</v>
       </c>
@@ -2084,16 +2177,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V76"/>
+  <dimension ref="A1:V80"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="K26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" style="7" customWidth="1"/>
@@ -2120,7 +2213,7 @@
     <col min="23" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="14.25" customHeight="1" thickBot="1">
+    <row r="1" spans="2:22" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -2140,7 +2233,7 @@
       </c>
       <c r="U1" s="12"/>
     </row>
-    <row r="2" spans="2:22" ht="16.5" customHeight="1" thickBot="1">
+    <row r="2" spans="2:22" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E2" s="67" t="s">
         <v>20</v>
       </c>
@@ -2164,7 +2257,7 @@
       </c>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="2:22" ht="14.25" customHeight="1" thickBot="1">
+    <row r="3" spans="2:22" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E3" s="70"/>
       <c r="F3" s="71"/>
       <c r="G3" s="71"/>
@@ -2182,9 +2275,9 @@
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
     </row>
-    <row r="4" spans="2:22" ht="12.75" customHeight="1" thickBot="1">
+    <row r="4" spans="2:22" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E4" s="58" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
@@ -2204,7 +2297,7 @@
       <c r="T4" s="19"/>
       <c r="U4" s="19"/>
     </row>
-    <row r="5" spans="2:22">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="61"/>
@@ -2224,7 +2317,7 @@
       <c r="T5" s="19"/>
       <c r="U5" s="19"/>
     </row>
-    <row r="6" spans="2:22" s="21" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
+    <row r="6" spans="2:22" s="21" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="22"/>
       <c r="E6" s="64"/>
       <c r="F6" s="65"/>
@@ -2244,7 +2337,7 @@
       <c r="U6" s="24"/>
       <c r="V6" s="25"/>
     </row>
-    <row r="7" spans="2:22" s="31" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
+    <row r="7" spans="2:22" s="31" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>21</v>
       </c>
@@ -2306,28 +2399,38 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:22" s="39" customFormat="1" ht="27">
+    <row r="8" spans="2:22" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="32">
         <v>1</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="34" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H8" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
+      <c r="I8" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
+      <c r="L8" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M8" s="36"/>
-      <c r="N8" s="35"/>
+      <c r="N8" s="35">
+        <v>2</v>
+      </c>
       <c r="O8" s="34"/>
       <c r="P8" s="37">
         <v>43712</v>
@@ -2340,26 +2443,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:22" s="39" customFormat="1" ht="15.75">
+    <row r="9" spans="2:22" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B9" s="40"/>
       <c r="C9" s="41" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H9" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
+      <c r="I9" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M9" s="36"/>
       <c r="N9" s="35"/>
       <c r="O9" s="34"/>
@@ -2374,26 +2487,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:22" s="39" customFormat="1" ht="15.75">
+    <row r="10" spans="2:22" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B10" s="40"/>
       <c r="C10" s="41" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H10" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
+      <c r="I10" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M10" s="36"/>
       <c r="N10" s="35"/>
       <c r="O10" s="34"/>
@@ -2408,26 +2531,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:22" s="39" customFormat="1" ht="15.75">
+    <row r="11" spans="2:22" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B11" s="40"/>
       <c r="C11" s="41" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H11" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
+      <c r="I11" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="L11" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M11" s="36"/>
       <c r="N11" s="35"/>
       <c r="O11" s="34"/>
@@ -2442,26 +2575,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:22" s="39" customFormat="1" ht="15.75">
+    <row r="12" spans="2:22" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B12" s="40"/>
       <c r="C12" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E12" s="53"/>
       <c r="F12" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="54"/>
+        <v>48</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H12" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="55"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
+      <c r="I12" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M12" s="54"/>
       <c r="N12" s="53"/>
       <c r="O12" s="52"/>
@@ -2476,26 +2619,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:22" s="39" customFormat="1" ht="25.5">
+    <row r="13" spans="2:22" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B13" s="40"/>
       <c r="C13" s="41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="54"/>
+        <v>49</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H13" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="55"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
+      <c r="I13" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M13" s="54"/>
       <c r="N13" s="53"/>
       <c r="O13" s="52"/>
@@ -2510,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:22" s="39" customFormat="1" ht="15.75">
+    <row r="14" spans="2:22" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B14" s="40">
         <v>2</v>
       </c>
@@ -2520,18 +2673,30 @@
       </c>
       <c r="E14" s="35"/>
       <c r="F14" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H14" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
+      <c r="I14" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="L14" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M14" s="36"/>
-      <c r="N14" s="35"/>
+      <c r="N14" s="35">
+        <v>1</v>
+      </c>
       <c r="O14" s="34"/>
       <c r="P14" s="37">
         <v>43712</v>
@@ -2544,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:22" s="39" customFormat="1" ht="15.75">
+    <row r="15" spans="2:22" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B15" s="40"/>
       <c r="C15" s="41" t="s">
         <v>34</v>
@@ -2554,16 +2719,26 @@
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H15" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="42"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
+      <c r="I15" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M15" s="36"/>
       <c r="N15" s="35"/>
       <c r="O15" s="34"/>
@@ -2576,26 +2751,36 @@
       <c r="T15" s="34"/>
       <c r="U15" s="36"/>
     </row>
-    <row r="16" spans="2:22" s="39" customFormat="1" ht="40.5">
+    <row r="16" spans="2:22" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B16" s="40"/>
       <c r="C16" s="41" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H16" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
+      <c r="I16" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M16" s="36"/>
       <c r="N16" s="35"/>
       <c r="O16" s="34"/>
@@ -2608,31 +2793,45 @@
       <c r="T16" s="34"/>
       <c r="U16" s="36"/>
     </row>
-    <row r="17" spans="1:21" s="39" customFormat="1" ht="15.75">
+    <row r="17" spans="1:21" s="39" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B17" s="40">
         <v>3</v>
       </c>
       <c r="C17" s="41"/>
       <c r="D17" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="35"/>
+        <v>50</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>87</v>
+      </c>
       <c r="F17" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H17" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
+      <c r="I17" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="L17" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M17" s="36"/>
-      <c r="N17" s="35"/>
+      <c r="N17" s="35">
+        <v>2</v>
+      </c>
       <c r="O17" s="34"/>
       <c r="P17" s="37">
         <v>43712</v>
@@ -2645,28 +2844,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="39" customFormat="1" ht="27">
+    <row r="18" spans="1:21" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B18" s="40">
         <v>4</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="35"/>
+        <v>62</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>88</v>
+      </c>
       <c r="F18" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H18" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
+      <c r="I18" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="L18" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M18" s="36"/>
-      <c r="N18" s="35"/>
+      <c r="N18" s="35">
+        <v>6</v>
+      </c>
       <c r="O18" s="34"/>
       <c r="P18" s="37">
         <v>43712</v>
@@ -2679,64 +2892,82 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="39" customFormat="1" ht="27">
-      <c r="B19" s="40">
+    <row r="19" spans="1:21" s="39" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B19" s="40"/>
+      <c r="C19" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="54"/>
+      <c r="L19" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M19" s="54"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
+      <c r="T19" s="52"/>
+      <c r="U19" s="54"/>
+    </row>
+    <row r="20" spans="1:21" s="39" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B20" s="40">
         <v>5</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="56">
-        <v>43712</v>
-      </c>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" s="39" customFormat="1" ht="27">
-      <c r="B20" s="40">
-        <v>6</v>
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="35"/>
+        <v>63</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>90</v>
+      </c>
       <c r="F20" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H20" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
+        <v>32</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="L20" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M20" s="36"/>
       <c r="N20" s="35"/>
       <c r="O20" s="34"/>
-      <c r="P20" s="37">
+      <c r="P20" s="56">
         <v>43712</v>
       </c>
       <c r="Q20" s="36"/>
@@ -2747,30 +2978,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="39" customFormat="1" ht="15.75">
+    <row r="21" spans="1:21" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B21" s="40">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="41"/>
       <c r="D21" s="34" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E21" s="35"/>
       <c r="F21" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H21" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
+      <c r="I21" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="L21" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M21" s="36"/>
       <c r="N21" s="35"/>
       <c r="O21" s="34"/>
-      <c r="P21" s="56">
+      <c r="P21" s="37">
         <v>43712</v>
       </c>
       <c r="Q21" s="36"/>
@@ -2781,30 +3022,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="39" customFormat="1" ht="15.75">
+    <row r="22" spans="1:21" s="39" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B22" s="40">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="41"/>
-      <c r="D22" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="35"/>
+      <c r="D22" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>91</v>
+      </c>
       <c r="F22" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>83</v>
+      </c>
       <c r="H22" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
+        <v>33</v>
+      </c>
+      <c r="I22" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="L22" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M22" s="36"/>
       <c r="N22" s="35"/>
       <c r="O22" s="34"/>
-      <c r="P22" s="37"/>
+      <c r="P22" s="56">
+        <v>43712</v>
+      </c>
       <c r="Q22" s="36"/>
       <c r="R22" s="36"/>
       <c r="S22" s="36"/>
@@ -2813,24 +3068,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="39" customFormat="1" ht="15.75">
+    <row r="23" spans="1:21" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B23" s="40">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="41"/>
-      <c r="D23" s="34" t="s">
-        <v>58</v>
+      <c r="D23" s="51" t="s">
+        <v>66</v>
       </c>
       <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
+      <c r="F23" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="L23" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M23" s="36"/>
-      <c r="N23" s="35"/>
+      <c r="N23" s="35">
+        <v>6</v>
+      </c>
       <c r="O23" s="34"/>
       <c r="P23" s="37"/>
       <c r="Q23" s="36"/>
@@ -2841,22 +3112,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="39" customFormat="1" ht="27">
+    <row r="24" spans="1:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B24" s="40">
-        <v>10</v>
-      </c>
-      <c r="C24" s="41"/>
+        <v>9</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="D24" s="34" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
+      <c r="F24" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="J24" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="L24" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M24" s="36"/>
       <c r="N24" s="35"/>
       <c r="O24" s="34"/>
@@ -2869,107 +3156,161 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="39" customFormat="1" ht="40.5">
-      <c r="B25" s="40">
+    <row r="25" spans="1:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="53"/>
+      <c r="F25" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K25" s="54"/>
+      <c r="L25" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M25" s="54"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="P25" s="56"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="54"/>
+      <c r="T25" s="52"/>
+      <c r="U25" s="54"/>
+    </row>
+    <row r="26" spans="1:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="53"/>
+      <c r="F26" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="J26" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" s="54"/>
+      <c r="L26" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M26" s="54"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="54"/>
+      <c r="T26" s="52"/>
+      <c r="U26" s="54"/>
+    </row>
+    <row r="27" spans="1:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B27" s="40">
+        <v>10</v>
+      </c>
+      <c r="C27" s="41"/>
+      <c r="D27" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="53"/>
+      <c r="F27" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H27" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K27" s="54"/>
+      <c r="L27" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M27" s="54"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="54"/>
+      <c r="T27" s="52"/>
+      <c r="U27" s="54"/>
+    </row>
+    <row r="28" spans="1:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B28" s="40">
         <v>11</v>
-      </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" s="39" customFormat="1" ht="27">
-      <c r="B26" s="40">
-        <v>12</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="36"/>
-      <c r="R26" s="36"/>
-      <c r="S26" s="36"/>
-      <c r="T26" s="38"/>
-      <c r="U26" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" s="39" customFormat="1" ht="15.75">
-      <c r="B27" s="40">
-        <v>13</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="36"/>
-      <c r="R27" s="36"/>
-      <c r="S27" s="36"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" s="39" customFormat="1" ht="27">
-      <c r="B28" s="40">
-        <v>14</v>
       </c>
       <c r="C28" s="41"/>
       <c r="D28" s="34" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
+      <c r="F28" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J28" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="L28" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M28" s="36"/>
       <c r="N28" s="35"/>
-      <c r="O28" s="34"/>
+      <c r="O28" s="34" t="s">
+        <v>94</v>
+      </c>
       <c r="P28" s="37"/>
       <c r="Q28" s="36"/>
       <c r="R28" s="36"/>
@@ -2979,24 +3320,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="39" customFormat="1" ht="15.75">
+    <row r="29" spans="1:21" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B29" s="40">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="34" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
+      <c r="F29" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J29" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K29" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="L29" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M29" s="36"/>
-      <c r="N29" s="35"/>
+      <c r="N29" s="35">
+        <v>2</v>
+      </c>
       <c r="O29" s="34"/>
       <c r="P29" s="37"/>
       <c r="Q29" s="36"/>
@@ -3007,25 +3364,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="39" customFormat="1" ht="27">
+    <row r="30" spans="1:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B30" s="40">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C30" s="41"/>
       <c r="D30" s="34" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
+      <c r="F30" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H30" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K30" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="L30" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M30" s="36"/>
       <c r="N30" s="35"/>
-      <c r="O30" s="34"/>
+      <c r="O30" s="34" t="s">
+        <v>95</v>
+      </c>
       <c r="P30" s="37"/>
       <c r="Q30" s="36"/>
       <c r="R30" s="36"/>
@@ -3035,25 +3408,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="39" customFormat="1" ht="15.75">
+    <row r="31" spans="1:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B31" s="40">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C31" s="41"/>
       <c r="D31" s="34" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
+      <c r="F31" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31" s="36" t="s">
+        <v>86</v>
+      </c>
       <c r="M31" s="36"/>
       <c r="N31" s="35"/>
-      <c r="O31" s="34"/>
+      <c r="O31" s="34" t="s">
+        <v>96</v>
+      </c>
       <c r="P31" s="37"/>
       <c r="Q31" s="36"/>
       <c r="R31" s="36"/>
@@ -3063,169 +3452,231 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="39" customFormat="1" ht="15.75">
+    <row r="32" spans="1:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B32" s="40">
+        <v>15</v>
+      </c>
+      <c r="C32" s="41"/>
+      <c r="D32" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="J32" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K32" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="L32" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M32" s="54"/>
+      <c r="N32" s="53">
+        <v>6</v>
+      </c>
+      <c r="O32" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="54"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="54"/>
+      <c r="T32" s="52"/>
+      <c r="U32" s="54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B33" s="40">
+        <v>16</v>
+      </c>
+      <c r="C33" s="41"/>
+      <c r="D33" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="53"/>
+      <c r="F33" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="L33" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M33" s="54"/>
+      <c r="N33" s="53">
+        <v>6</v>
+      </c>
+      <c r="O33" s="52"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="54"/>
+      <c r="R33" s="54"/>
+      <c r="S33" s="54"/>
+      <c r="T33" s="52"/>
+      <c r="U33" s="54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B34" s="40">
+        <v>17</v>
+      </c>
+      <c r="C34" s="41"/>
+      <c r="D34" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="53"/>
+      <c r="F34" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H34" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K34" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="L34" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M34" s="54"/>
+      <c r="N34" s="53"/>
+      <c r="O34" s="52"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="54"/>
+      <c r="R34" s="54"/>
+      <c r="S34" s="54"/>
+      <c r="T34" s="52"/>
+      <c r="U34" s="54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B35" s="40">
         <v>18</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="38"/>
-      <c r="U32" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B33" s="40">
+      <c r="C35" s="41"/>
+      <c r="D35" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="53"/>
+      <c r="F35" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="J35" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="K35" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="L35" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M35" s="54"/>
+      <c r="N35" s="53"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="54"/>
+      <c r="R35" s="54"/>
+      <c r="S35" s="54"/>
+      <c r="T35" s="52"/>
+      <c r="U35" s="54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B36" s="40">
         <v>19</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="36"/>
-      <c r="S33" s="36"/>
-      <c r="T33" s="38"/>
-      <c r="U33" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B34" s="40">
+      <c r="C36" s="41"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="81"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="81"/>
+      <c r="L36" s="81"/>
+      <c r="M36" s="81"/>
+      <c r="N36" s="81"/>
+      <c r="O36" s="81"/>
+      <c r="P36" s="83"/>
+      <c r="Q36" s="81"/>
+      <c r="R36" s="81"/>
+      <c r="S36" s="81"/>
+      <c r="T36" s="52"/>
+      <c r="U36" s="81"/>
+    </row>
+    <row r="37" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B37" s="40">
         <v>20</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="34"/>
-      <c r="P34" s="37"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="36"/>
-      <c r="S34" s="36"/>
-      <c r="T34" s="38"/>
-      <c r="U34" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B35" s="40">
+      <c r="C37" s="41"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="81"/>
+      <c r="L37" s="81"/>
+      <c r="M37" s="81"/>
+      <c r="N37" s="81"/>
+      <c r="O37" s="81"/>
+      <c r="P37" s="83"/>
+      <c r="Q37" s="81"/>
+      <c r="R37" s="81"/>
+      <c r="S37" s="81"/>
+      <c r="T37" s="52"/>
+      <c r="U37" s="81"/>
+    </row>
+    <row r="38" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B38" s="40">
         <v>21</v>
-      </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="34"/>
-      <c r="P35" s="37"/>
-      <c r="Q35" s="36"/>
-      <c r="R35" s="36"/>
-      <c r="S35" s="36"/>
-      <c r="T35" s="38"/>
-      <c r="U35" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B36" s="40">
-        <v>22</v>
-      </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="37"/>
-      <c r="Q36" s="36"/>
-      <c r="R36" s="36"/>
-      <c r="S36" s="36"/>
-      <c r="T36" s="38"/>
-      <c r="U36" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B37" s="40">
-        <v>23</v>
-      </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="35"/>
-      <c r="O37" s="34"/>
-      <c r="P37" s="37"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="T37" s="38"/>
-      <c r="U37" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B38" s="40">
-        <v>24</v>
       </c>
       <c r="C38" s="41"/>
       <c r="D38" s="34"/>
@@ -3249,9 +3700,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="39" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B39" s="40">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C39" s="41"/>
       <c r="D39" s="34"/>
@@ -3275,9 +3726,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="40" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B40" s="40">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C40" s="41"/>
       <c r="D40" s="34"/>
@@ -3301,9 +3752,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="41" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B41" s="40">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="34"/>
@@ -3327,9 +3778,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="42" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B42" s="40">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C42" s="41"/>
       <c r="D42" s="34"/>
@@ -3353,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="43" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B43" s="40">
         <v>29</v>
       </c>
@@ -3379,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="44" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B44" s="40">
         <v>30</v>
       </c>
@@ -3405,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="45" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B45" s="40">
         <v>31</v>
       </c>
@@ -3431,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="46" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B46" s="40">
         <v>32</v>
       </c>
@@ -3457,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="47" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B47" s="40">
         <v>33</v>
       </c>
@@ -3483,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="48" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B48" s="40">
         <v>34</v>
       </c>
@@ -3509,7 +3960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="49" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B49" s="40">
         <v>35</v>
       </c>
@@ -3535,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="50" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B50" s="40">
         <v>36</v>
       </c>
@@ -3561,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="51" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B51" s="40">
         <v>37</v>
       </c>
@@ -3587,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="52" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B52" s="40">
         <v>38</v>
       </c>
@@ -3613,7 +4064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="53" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B53" s="40">
         <v>39</v>
       </c>
@@ -3639,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="54" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B54" s="40">
         <v>40</v>
       </c>
@@ -3665,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="55" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B55" s="40">
         <v>41</v>
       </c>
@@ -3691,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="56" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B56" s="40">
         <v>42</v>
       </c>
@@ -3717,7 +4168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="57" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B57" s="40">
         <v>43</v>
       </c>
@@ -3743,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="58" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B58" s="40">
         <v>44</v>
       </c>
@@ -3769,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="59" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B59" s="40">
         <v>45</v>
       </c>
@@ -3795,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="60" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B60" s="40">
         <v>46</v>
       </c>
@@ -3821,7 +4272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="61" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B61" s="40">
         <v>47</v>
       </c>
@@ -3847,7 +4298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="62" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B62" s="40">
         <v>48</v>
       </c>
@@ -3873,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="63" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B63" s="40">
         <v>49</v>
       </c>
@@ -3899,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="64" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B64" s="40">
         <v>50</v>
       </c>
@@ -3925,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="65" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B65" s="40">
         <v>51</v>
       </c>
@@ -3951,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="66" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B66" s="40">
         <v>52</v>
       </c>
@@ -3977,7 +4428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="67" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B67" s="40">
         <v>53</v>
       </c>
@@ -4003,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="68" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B68" s="40">
         <v>54</v>
       </c>
@@ -4029,7 +4480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="69" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B69" s="40">
         <v>55</v>
       </c>
@@ -4055,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="70" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B70" s="40">
         <v>56</v>
       </c>
@@ -4081,7 +4532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="71" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B71" s="40">
         <v>57</v>
       </c>
@@ -4107,7 +4558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="72" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B72" s="40">
         <v>58</v>
       </c>
@@ -4133,7 +4584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="73" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B73" s="40">
         <v>59</v>
       </c>
@@ -4159,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="74" spans="2:21" s="39" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B74" s="40">
         <v>60</v>
       </c>
@@ -4185,34 +4636,122 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:21" s="39" customFormat="1" ht="16.5" thickBot="1">
+    <row r="75" spans="2:21" s="39" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B75" s="43">
         <v>61</v>
       </c>
       <c r="C75" s="44"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="46"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="47"/>
-      <c r="H75" s="47"/>
-      <c r="I75" s="47"/>
-      <c r="J75" s="47"/>
-      <c r="K75" s="47"/>
-      <c r="L75" s="47"/>
-      <c r="M75" s="47"/>
-      <c r="N75" s="46"/>
-      <c r="O75" s="45"/>
-      <c r="P75" s="48"/>
-      <c r="Q75" s="47"/>
-      <c r="R75" s="47"/>
-      <c r="S75" s="47"/>
-      <c r="T75" s="49"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="35"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="36"/>
+      <c r="I75" s="36"/>
+      <c r="J75" s="36"/>
+      <c r="K75" s="36"/>
+      <c r="L75" s="36"/>
+      <c r="M75" s="36"/>
+      <c r="N75" s="35"/>
+      <c r="O75" s="34"/>
+      <c r="P75" s="37"/>
+      <c r="Q75" s="36"/>
+      <c r="R75" s="36"/>
+      <c r="S75" s="36"/>
+      <c r="T75" s="38"/>
       <c r="U75" s="36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:21">
-      <c r="N76" s="12"/>
+    <row r="76" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D76" s="34"/>
+      <c r="E76" s="35"/>
+      <c r="F76" s="36"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="36"/>
+      <c r="I76" s="36"/>
+      <c r="J76" s="36"/>
+      <c r="K76" s="36"/>
+      <c r="L76" s="36"/>
+      <c r="M76" s="36"/>
+      <c r="N76" s="35"/>
+      <c r="O76" s="34"/>
+      <c r="P76" s="37"/>
+      <c r="Q76" s="36"/>
+      <c r="R76" s="36"/>
+      <c r="S76" s="36"/>
+      <c r="T76" s="38"/>
+      <c r="U76" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D77" s="34"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="36"/>
+      <c r="I77" s="36"/>
+      <c r="J77" s="36"/>
+      <c r="K77" s="36"/>
+      <c r="L77" s="36"/>
+      <c r="M77" s="36"/>
+      <c r="N77" s="35"/>
+      <c r="O77" s="34"/>
+      <c r="P77" s="37"/>
+      <c r="Q77" s="36"/>
+      <c r="R77" s="36"/>
+      <c r="S77" s="36"/>
+      <c r="T77" s="38"/>
+      <c r="U77" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D78" s="34"/>
+      <c r="E78" s="35"/>
+      <c r="F78" s="36"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="36"/>
+      <c r="I78" s="36"/>
+      <c r="J78" s="36"/>
+      <c r="K78" s="36"/>
+      <c r="L78" s="36"/>
+      <c r="M78" s="36"/>
+      <c r="N78" s="35"/>
+      <c r="O78" s="34"/>
+      <c r="P78" s="37"/>
+      <c r="Q78" s="36"/>
+      <c r="R78" s="36"/>
+      <c r="S78" s="36"/>
+      <c r="T78" s="38"/>
+      <c r="U78" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="45"/>
+      <c r="E79" s="46"/>
+      <c r="F79" s="47"/>
+      <c r="G79" s="47"/>
+      <c r="H79" s="47"/>
+      <c r="I79" s="47"/>
+      <c r="J79" s="47"/>
+      <c r="K79" s="47"/>
+      <c r="L79" s="47"/>
+      <c r="M79" s="47"/>
+      <c r="N79" s="46"/>
+      <c r="O79" s="45"/>
+      <c r="P79" s="48"/>
+      <c r="Q79" s="47"/>
+      <c r="R79" s="47"/>
+      <c r="S79" s="47"/>
+      <c r="T79" s="49"/>
+      <c r="U79" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="N80" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4225,13 +4764,13 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U75" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U38:U79 U8:U35" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I75" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I38:I79 I8:I35" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H75" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H38:H79 H8:H35" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>